<commit_message>
Added 'K' instead of e-3 to x axis
</commit_message>
<xml_diff>
--- a/MDD-GWAS.xlsx
+++ b/MDD-GWAS.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mcintosh/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mcintosh/Documents/Projects/R-Projects/MDD GWAS Progress/MDD GWAS/MDD-GWAS-Progress/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{1CD3B523-8BAE-2E43-ADB1-F5A2A149797E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2499FA06-36B6-7D48-8948-FF207F1712F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5580" yWindow="2300" windowWidth="27640" windowHeight="16940" xr2:uid="{18275BCD-E0EA-CA4C-A0F6-D8B3A799BC9E}"/>
+    <workbookView xWindow="2600" yWindow="1300" windowWidth="27640" windowHeight="16940" xr2:uid="{18275BCD-E0EA-CA4C-A0F6-D8B3A799BC9E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -57,9 +57,6 @@
     <t>26176920</t>
   </si>
   <si>
-    <t>Converge</t>
-  </si>
-  <si>
     <t>Wray</t>
   </si>
   <si>
@@ -88,6 +85,9 @@
   </si>
   <si>
     <t>34045744</t>
+  </si>
+  <si>
+    <t>CONVERGE</t>
   </si>
 </sst>
 </file>
@@ -451,7 +451,7 @@
   <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -473,7 +473,7 @@
         <v>3</v>
       </c>
       <c r="E1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
@@ -484,7 +484,7 @@
         <v>2013</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D2">
         <v>0</v>
@@ -495,7 +495,7 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>7</v>
+        <v>17</v>
       </c>
       <c r="B3">
         <v>2015</v>
@@ -518,7 +518,7 @@
         <v>2016</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D4">
         <v>15</v>
@@ -529,13 +529,13 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B5">
         <v>2018</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D5">
         <v>44</v>
@@ -546,13 +546,13 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B6">
         <v>2019</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D6">
         <v>102</v>
@@ -563,13 +563,13 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B7">
         <v>2021</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D7">
         <v>178</v>
@@ -580,7 +580,7 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B8">
         <v>2022</v>

</xml_diff>

<commit_message>
Add PGC* to 3 studies
</commit_message>
<xml_diff>
--- a/MDD-GWAS.xlsx
+++ b/MDD-GWAS.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mcintosh/Documents/Projects/R-Projects/MDD GWAS Progress/MDD GWAS/MDD-GWAS-Progress/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2499FA06-36B6-7D48-8948-FF207F1712F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{435039BE-565D-D14D-89A0-BAE3925AFFBA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2600" yWindow="1300" windowWidth="27640" windowHeight="16940" xr2:uid="{18275BCD-E0EA-CA4C-A0F6-D8B3A799BC9E}"/>
   </bookViews>
@@ -48,18 +48,12 @@
     <t>Nhits</t>
   </si>
   <si>
-    <t>Ripke</t>
-  </si>
-  <si>
     <t>Hyde</t>
   </si>
   <si>
     <t>26176920</t>
   </si>
   <si>
-    <t>Wray</t>
-  </si>
-  <si>
     <t xml:space="preserve">Howard </t>
   </si>
   <si>
@@ -72,9 +66,6 @@
     <t>30718901</t>
   </si>
   <si>
-    <t>PGC3</t>
-  </si>
-  <si>
     <t>22472876</t>
   </si>
   <si>
@@ -88,6 +79,15 @@
   </si>
   <si>
     <t>CONVERGE</t>
+  </si>
+  <si>
+    <t>Ripke (PGC1)</t>
+  </si>
+  <si>
+    <t>Wray (PGC2)</t>
+  </si>
+  <si>
+    <t>Adams (PGC3)</t>
   </si>
 </sst>
 </file>
@@ -451,7 +451,7 @@
   <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -473,18 +473,18 @@
         <v>3</v>
       </c>
       <c r="E1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>4</v>
+        <v>15</v>
       </c>
       <c r="B2">
         <v>2013</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="D2">
         <v>0</v>
@@ -495,13 +495,13 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B3">
         <v>2015</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D3">
         <v>2</v>
@@ -512,13 +512,13 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B4">
         <v>2016</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="D4">
         <v>15</v>
@@ -529,13 +529,13 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="B5">
         <v>2018</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D5">
         <v>44</v>
@@ -546,13 +546,13 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B6">
         <v>2019</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D6">
         <v>102</v>
@@ -563,13 +563,13 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="B7">
         <v>2021</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="D7">
         <v>178</v>
@@ -580,7 +580,7 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="B8">
         <v>2022</v>

</xml_diff>